<commit_message>
Revert "Merge remote-tracking branch 'origin/branch1' into branch1"
This reverts commit fd46323c32dc352367210f07fffcccb62005d6b3.
</commit_message>
<xml_diff>
--- a/Branch1.xlsx
+++ b/Branch1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JonasSchneider/Documents/Sonstiges/Git/Git_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E8028F-0303-1E4E-9DEC-AC1C4C1F1C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E37D869-CBBA-0A42-B342-0670C86E2355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5080" yWindow="1900" windowWidth="28240" windowHeight="17240" xr2:uid="{7CF3549C-A9AF-B547-96A0-0D57D4863DC9}"/>
   </bookViews>
@@ -382,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35DD00C2-0A06-6A46-A3E3-68A6B7A5DF20}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -405,11 +405,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>